<commit_message>
update code search feature
</commit_message>
<xml_diff>
--- a/OWASP_JUICE_SHOP_SEARCH_FEATURES_CYPRESS_TESTING_FINAL (1).xlsx
+++ b/OWASP_JUICE_SHOP_SEARCH_FEATURES_CYPRESS_TESTING_FINAL (1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="17580"/>
+    <workbookView windowHeight="17580"/>
   </bookViews>
   <sheets>
     <sheet name="Search Test Cases" sheetId="1" r:id="rId1"/>
@@ -1665,8 +1665,8 @@
   <sheetPr/>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Update Juice Shop Cypress testing Excel file
Replaces the previous version of the OWASP_JUICE_SHOP_SEARCH_FEATURES_CYPRESS_TESTING_FINAL (1).xlsx file with an updated binary. Details of the changes are not visible in the diff.
</commit_message>
<xml_diff>
--- a/OWASP_JUICE_SHOP_SEARCH_FEATURES_CYPRESS_TESTING_FINAL (1).xlsx
+++ b/OWASP_JUICE_SHOP_SEARCH_FEATURES_CYPRESS_TESTING_FINAL (1).xlsx
@@ -360,8 +360,7 @@
     <t>Kiểm thử tìm kiếm có dấu cách ở hai đầu</t>
   </si>
   <si>
-    <t>1. Nhấn vào icon tìm kiếm
-2. Nhập ' apple ' vào ô tìm kiếm và nhấn Enter</t>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve"> apple </t>
@@ -607,7 +606,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -623,12 +622,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1127,7 +1120,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1151,16 +1144,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1169,85 +1162,85 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1290,16 +1283,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1320,7 +1313,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1678,7 +1671,7 @@
   <sheetPr/>
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>